<commit_message>
12/01/2015 11.21 Signed-off-by: cyrexxx <kartik@kth.se>
</commit_message>
<xml_diff>
--- a/Exjobb_xml/VOCvsVmppt.xlsx
+++ b/Exjobb_xml/VOCvsVmppt.xlsx
@@ -80,10 +80,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="144"/>
+      <c14:style val="112"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="44"/>
+      <c:style val="12"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -108,7 +108,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.0724443758255709E-2"/>
+          <c:y val="7.7241454285669919E-2"/>
+          <c:w val="0.849433208103889"/>
+          <c:h val="0.87756392607997691"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -133,7 +143,6 @@
             <c:trendlineType val="linear"/>
             <c:forward val="1"/>
             <c:backward val="3"/>
-            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -529,13 +538,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185047680"/>
-        <c:axId val="185045376"/>
+        <c:axId val="88563712"/>
+        <c:axId val="88565632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185047680"/>
+        <c:axId val="88563712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -562,12 +572,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185045376"/>
+        <c:crossAx val="88565632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185045376"/>
+        <c:axId val="88565632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185047680"/>
+        <c:crossAx val="88563712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -614,8 +624,565 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.25" r="0.25" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup paperSize="9" orientation="portrait"/>
+    <c:pageSetup paperSize="8" orientation="landscape"/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="112"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="12"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Voc Vs Vmppt</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.0724443758255709E-2"/>
+          <c:y val="7.7241454285669919E-2"/>
+          <c:w val="0.849433208103889"/>
+          <c:h val="0.87756392607997691"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V_mpp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:forward val="1"/>
+            <c:backward val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2.76810999999983</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0939694082233999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2613356894425598</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3662997740859</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4439819209679601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.50365713437805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5522563734455299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5936376652889699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6302176472113299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6623999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6903731488220402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7148646995922099</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.7367370534121598</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7568526113835699</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7760737149338799</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7949339027463602</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.81286742374831</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8290790618084198</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8430255888159901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8558042973104598</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.8820880568901801</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9076959012257801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.9295756331699199</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.94749485059863</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9638249572411901</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.9802566095919198</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.9967428827272098</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.0130017455696301</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.0287511670417304</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.0437091160660801</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.0576196949171299</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.0704967965368999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.0825134758850803</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.0938448450657097</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.1046660161827901</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.1151474894617204</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.1253536919196501</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.1352429773655102</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.14476908772959</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.1538857649421699</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.1625476889483197</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1707460050174001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.1785192281647898</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.1859090392057103</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.1929571189554</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.1997051482290901</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.2061948078420004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.2124677786093798</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.2185657413464597</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.2245303768684597</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.2304014311871798</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.23619867614818</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.2419300999107401</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.24760353833181</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.2532268272683504</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.2588078025773299</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.2643543001156896</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.2698741557403901</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.2753752053084</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.2808652846766604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2.1395198701023102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4706073158181598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6187705578089999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6915964410223099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7595614852591299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8540095141996602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8839136951073199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.94245634408191</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.94245634408191</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.00221885383734</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0216663406048001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0996303263018401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.1160636437217701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.13478700931487</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1597247229936198</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1550039258151101</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.1662591949765799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2100938579447198</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2339597591731701</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.2424563440819099</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2424563440819099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.2424563440819099</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2828003889218502</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.3132723343332202</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.3528361946387402</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3536131284543602</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.3545994498678402</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.35599823338895</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.3716066657227999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3711987128388401</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.3913422318328901</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3971306261249099</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4122574564788901</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.41444384736179</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.44245634408191</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.44245634408191</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.4627443374298101</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4700183374772</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.4725040210411402</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.4750176455664898</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.50075380695043</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.5032919016565498</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.5057954002420701</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.5082079855253001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.52205089086215</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.5288578851516901</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.5424563440819101</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.56516297078347</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.5807855381359102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="121276672"/>
+        <c:axId val="132520576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="121276672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Voc</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132520576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="132520576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Vmppt</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121276672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.25" r="0.25" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="8" orientation="landscape"/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -652,6 +1219,215 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>71543</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.41219</cdr:x>
+      <cdr:y>0.33303</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.75788</cdr:x>
+      <cdr:y>0.43718</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="19521765">
+          <a:off x="4805504" y="2358793"/>
+          <a:ext cx="4030302" cy="737684"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:shade val="30000"/>
+                <a:satMod val="115000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="accent1">
+                <a:shade val="67500"/>
+                <a:satMod val="115000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:shade val="100000"/>
+                <a:satMod val="115000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:scene3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prstMaterial="translucentPowder"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.14567</cdr:x>
+      <cdr:y>0.17391</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.71552</cdr:x>
+      <cdr:y>0.8288</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Connector 5"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="1698308" y="1219200"/>
+          <a:ext cx="6643687" cy="4591050"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18489</cdr:x>
+      <cdr:y>0.24457</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.75678</cdr:x>
+      <cdr:y>0.91304</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="13" name="Straight Connector 12"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="2155508" y="1714500"/>
+          <a:ext cx="6667502" cy="4686300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -943,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE17" sqref="AE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1630,11 +2406,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>